<commit_message>
US-10748 [IMP] MML/MSL: Added the info/placeholder info to the PO f/up, FO f/up, IR f/up, Product List, TKC, Kitting Order, RR Product List Consistency report, RR Inventory Review, Export Inventory Level, MSR, Consolidated MSR and Periodical forecast reports
</commit_message>
<xml_diff>
--- a/bin/addons/specific_rules/report/report_stock_inventory.xlsx
+++ b/bin/addons/specific_rules/report/report_stock_inventory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>DB/instance name</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>PCE</t>
+  </si>
+  <si>
+    <t>MML</t>
+  </si>
+  <si>
+    <t>MSL</t>
   </si>
 </sst>
 </file>
@@ -562,25 +568,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" customWidth="1"/>
-    <col min="13" max="15" width="15.28515625" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" customWidth="1"/>
+    <col min="3" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="13" width="15.28515625" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="15" max="17" width="15.28515625" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -591,7 +597,7 @@
       <c r="D1" s="8"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -602,7 +608,7 @@
       <c r="D2" s="11"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -613,7 +619,7 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -624,7 +630,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -635,7 +641,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -646,7 +652,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -657,7 +663,7 @@
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -668,7 +674,7 @@
       <c r="D8" s="8"/>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -679,7 +685,7 @@
       <c r="D9" s="8"/>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -695,12 +701,8 @@
       <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
         <v>4</v>
       </c>
@@ -731,8 +733,14 @@
       <c r="Q10" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -748,12 +756,8 @@
       <c r="E11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
         <v>4</v>
       </c>
@@ -784,8 +788,14 @@
       <c r="Q11" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -796,49 +806,55 @@
         <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>35</v>
       </c>
@@ -851,26 +867,26 @@
       <c r="D13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
+      <c r="E13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
       </c>
       <c r="I13" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J13" s="2">
         <v>0</v>
       </c>
       <c r="K13" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L13" s="2">
         <v>0</v>
@@ -887,7 +903,13 @@
       <c r="P13" s="2">
         <v>0</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="Q13" s="2">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="3">
         <v>4</v>
       </c>
     </row>

</xml_diff>